<commit_message>
Generic scaling is done & data changed a bit
</commit_message>
<xml_diff>
--- a/big_data2.xlsx
+++ b/big_data2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F470DC6D-C5E0-C44E-A965-480F6F79AA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E730C8F-DDDA-3448-ADC4-DB8D2F74F6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="2060" windowWidth="32200" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66:O66"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4376,13 +4376,13 @@
         <v>0</v>
       </c>
       <c r="J57" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K57" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L57" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M57">
         <v>0</v>
@@ -4438,13 +4438,13 @@
         <v>0</v>
       </c>
       <c r="J58" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K58" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L58" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M58">
         <v>30</v>
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H59" s="3">
         <v>10</v>
@@ -4553,7 +4553,7 @@
         <v>0</v>
       </c>
       <c r="G60" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H60" s="3">
         <v>10</v>
@@ -4615,7 +4615,7 @@
         <v>0</v>
       </c>
       <c r="G61" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H61" s="3">
         <v>10</v>
@@ -4677,7 +4677,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H62" s="3">
         <v>10</v>
@@ -4739,7 +4739,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H63" s="3">
         <v>10</v>
@@ -4801,7 +4801,7 @@
         <v>0</v>
       </c>
       <c r="G64" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H64" s="3">
         <v>10</v>
@@ -4863,7 +4863,7 @@
         <v>0</v>
       </c>
       <c r="G65" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H65" s="3">
         <v>10</v>
@@ -4872,13 +4872,13 @@
         <v>10</v>
       </c>
       <c r="J65" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K65" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L65" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M65">
         <v>30</v>
@@ -4925,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H66" s="3">
         <v>10</v>
@@ -4934,13 +4934,13 @@
         <v>10</v>
       </c>
       <c r="J66" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K66" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L66" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M66">
         <v>0</v>

</xml_diff>